<commit_message>
Adding results of running Budget KP with 10 percent budget on random datasets
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAC1AD4-E5EA-4EC5-AE98-855B162FF4D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C6D38D-BE4F-45E0-9B03-419BCDE0B8EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,9 +493,15 @@
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
+      <c r="E4">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="F4">
+        <v>0.96299999999999997</v>
+      </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.0000000000000027E-3</v>
       </c>
       <c r="J4">
         <f t="shared" si="2"/>
@@ -516,9 +522,15 @@
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.997</v>
+      </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.0000000000000027E-3</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
@@ -539,9 +551,15 @@
         <f t="shared" si="0"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="E6">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="F6">
+        <v>0.99299999999999999</v>
+      </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
@@ -562,9 +580,15 @@
         <f>ABS(B7-C7)</f>
         <v>1.0000000000000009E-2</v>
       </c>
+      <c r="E7">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.999</v>
+      </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0000000000000009E-2</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
@@ -585,9 +609,15 @@
         <f t="shared" ref="D8:D23" si="3">ABS(B8-C8)</f>
         <v>1.100000000000001E-2</v>
       </c>
+      <c r="E8">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="F8">
+        <v>0.97799999999999998</v>
+      </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.100000000000001E-2</v>
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
@@ -608,9 +638,15 @@
         <f t="shared" si="3"/>
         <v>5.0000000000000044E-3</v>
       </c>
+      <c r="E9">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.98899999999999999</v>
+      </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.0000000000000044E-3</v>
       </c>
       <c r="J9">
         <f t="shared" si="2"/>
@@ -631,9 +667,15 @@
         <f t="shared" si="3"/>
         <v>2.0000000000000018E-3</v>
       </c>
+      <c r="E10">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.98599999999999999</v>
+      </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0000000000000018E-3</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
@@ -654,6 +696,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E11">
+        <v>0.996</v>
+      </c>
+      <c r="F11">
+        <v>0.996</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -677,9 +725,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="E12">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="F12">
+        <v>0.97299999999999998</v>
+      </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
@@ -700,9 +754,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="E13">
+        <v>0.998</v>
+      </c>
+      <c r="F13">
+        <v>0.999</v>
+      </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="J13">
         <f t="shared" si="2"/>
@@ -723,9 +783,15 @@
         <f t="shared" si="3"/>
         <v>5.0000000000000044E-3</v>
       </c>
+      <c r="E14">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="F14">
+        <v>0.97699999999999998</v>
+      </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.0000000000000044E-3</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
@@ -746,9 +812,15 @@
         <f t="shared" si="3"/>
         <v>6.0000000000000053E-3</v>
       </c>
+      <c r="E15">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="F15">
+        <v>0.98199999999999998</v>
+      </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.0000000000000053E-3</v>
       </c>
       <c r="J15">
         <f t="shared" si="2"/>
@@ -769,9 +841,15 @@
         <f t="shared" si="3"/>
         <v>7.0000000000000062E-3</v>
       </c>
+      <c r="E16">
+        <v>0.98</v>
+      </c>
+      <c r="F16">
+        <v>0.97299999999999998</v>
+      </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.0000000000000062E-3</v>
       </c>
       <c r="J16">
         <f t="shared" si="2"/>
@@ -792,9 +870,15 @@
         <f t="shared" si="3"/>
         <v>6.0000000000000053E-3</v>
       </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.99399999999999999</v>
+      </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.0000000000000053E-3</v>
       </c>
       <c r="J17">
         <f t="shared" si="2"/>
@@ -815,9 +899,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="E18">
+        <v>0.997</v>
+      </c>
+      <c r="F18">
+        <v>0.998</v>
+      </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="J18">
         <f t="shared" si="2"/>
@@ -838,6 +928,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="E19">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="F19">
+        <v>0.94499999999999995</v>
+      </c>
       <c r="G19">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -861,9 +957,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="E20">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="F20">
+        <v>0.98699999999999999</v>
+      </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
@@ -884,9 +986,15 @@
         <f t="shared" si="3"/>
         <v>4.0000000000000036E-3</v>
       </c>
+      <c r="E21">
+        <v>0.997</v>
+      </c>
+      <c r="F21">
+        <v>0.99299999999999999</v>
+      </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.0000000000000036E-3</v>
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
@@ -907,9 +1015,15 @@
         <f t="shared" si="3"/>
         <v>3.0000000000000027E-3</v>
       </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0.997</v>
+      </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.0000000000000027E-3</v>
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
@@ -930,9 +1044,15 @@
         <f t="shared" si="3"/>
         <v>8.0000000000000071E-3</v>
       </c>
+      <c r="E23">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="F23">
+        <v>0.997</v>
+      </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.0000000000000071E-3</v>
       </c>
       <c r="J23">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Adding Budget Lily results to spreadsheet
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C6D38D-BE4F-45E0-9B03-419BCDE0B8EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F46E9D1-53EE-4D80-AE02-296AB3B1D28D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Data File Index</t>
   </si>
@@ -39,9 +39,6 @@
     <t>sonar</t>
   </si>
   <si>
-    <t>iris</t>
-  </si>
-  <si>
     <t>KP Training Acc</t>
   </si>
   <si>
@@ -67,6 +64,12 @@
   </si>
   <si>
     <t>KPD Testing Acc</t>
+  </si>
+  <si>
+    <t>iris 77/73</t>
+  </si>
+  <si>
+    <t>iris 113/37</t>
   </si>
 </sst>
 </file>
@@ -110,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,644 +422,690 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D6" si="0">ABS(B2-C2)</f>
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <f>ABS(E2-F2)</f>
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <f>ABS(H2-I2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
+      <c r="D2" s="2">
+        <f t="shared" ref="D2:D8" si="0">ABS(B2-C2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <f t="shared" ref="G2:G3" si="1">ABS(E2-F2)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <f t="shared" ref="J2:J3" si="2">ABS(H2-I2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G23" si="1">ABS(E3-F3)</f>
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J23" si="2">ABS(H3-I3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <f>ABS(E4-F4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <f>ABS(H4-I4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G25" si="3">ABS(E5-F5)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" ref="J5:J25" si="4">ABS(H5-I5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>0.96599999999999997</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>0.96299999999999997</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>0.96599999999999997</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>0.96299999999999997</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
+      <c r="G6">
+        <f t="shared" si="3"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>0.997</v>
       </c>
-      <c r="D5">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>0.997</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
+      <c r="G7">
+        <f t="shared" si="3"/>
         <v>3.0000000000000027E-3</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>0.99399999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>0.99299999999999999</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>0.99399999999999999</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>0.99299999999999999</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
+      <c r="G8">
+        <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="C7">
-        <v>0.999</v>
-      </c>
-      <c r="D7">
-        <f>ABS(B7-C7)</f>
-        <v>1.0000000000000009E-2</v>
-      </c>
-      <c r="E7">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="F7">
-        <v>0.999</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>1.0000000000000009E-2</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="C8">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ref="D8:D23" si="3">ABS(B8-C8)</f>
-        <v>1.100000000000001E-2</v>
-      </c>
-      <c r="E8">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="F8">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
-        <v>1.100000000000001E-2</v>
-      </c>
       <c r="J8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>0.98399999999999999</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="C9">
+        <v>0.999</v>
+      </c>
+      <c r="D9">
+        <f>ABS(B9-C9)</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="E9">
         <v>0.98899999999999999</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="3"/>
-        <v>5.0000000000000044E-3</v>
-      </c>
-      <c r="E9">
-        <v>0.98399999999999999</v>
-      </c>
       <c r="F9">
-        <v>0.98899999999999999</v>
+        <v>0.999</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000044E-3</v>
+        <f t="shared" si="3"/>
+        <v>1.0000000000000009E-2</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>0.98799999999999999</v>
+        <v>0.96699999999999997</v>
       </c>
       <c r="C10">
-        <v>0.98599999999999999</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
-        <v>2.0000000000000018E-3</v>
+        <f t="shared" ref="D10:D25" si="5">ABS(B10-C10)</f>
+        <v>1.100000000000001E-2</v>
       </c>
       <c r="E10">
-        <v>0.98799999999999999</v>
+        <v>0.96699999999999997</v>
       </c>
       <c r="F10">
-        <v>0.98599999999999999</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
-        <v>2.0000000000000018E-3</v>
+        <f t="shared" si="3"/>
+        <v>1.100000000000001E-2</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>0.996</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="C11">
-        <v>0.996</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000044E-3</v>
       </c>
       <c r="E11">
-        <v>0.996</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="F11">
-        <v>0.996</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>5.0000000000000044E-3</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>0.97399999999999998</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="C12">
-        <v>0.97299999999999998</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
-        <v>1.0000000000000009E-3</v>
+        <f t="shared" si="5"/>
+        <v>2.0000000000000018E-3</v>
       </c>
       <c r="E12">
-        <v>0.97399999999999998</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F12">
-        <v>0.97299999999999998</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>1.0000000000000009E-3</v>
+        <f t="shared" si="3"/>
+        <v>2.0000000000000018E-3</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>0.998</v>
+        <v>0.996</v>
       </c>
       <c r="C13">
-        <v>0.999</v>
+        <v>0.996</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
-        <v>1.0000000000000009E-3</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0.998</v>
+        <v>0.996</v>
       </c>
       <c r="F13">
-        <v>0.999</v>
+        <v>0.996</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>1.0000000000000009E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>0.98199999999999998</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="C14">
-        <v>0.97699999999999998</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="D14">
-        <f t="shared" si="3"/>
-        <v>5.0000000000000044E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="E14">
-        <v>0.98199999999999998</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="F14">
-        <v>0.97699999999999998</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000044E-3</v>
+        <f t="shared" si="3"/>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15">
-        <v>0.98799999999999999</v>
+        <v>0.998</v>
       </c>
       <c r="C15">
-        <v>0.98199999999999998</v>
+        <v>0.999</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
-        <v>6.0000000000000053E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="E15">
-        <v>0.98799999999999999</v>
+        <v>0.998</v>
       </c>
       <c r="F15">
-        <v>0.98199999999999998</v>
+        <v>0.999</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>6.0000000000000053E-3</v>
+        <f t="shared" si="3"/>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="J15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16">
-        <v>0.98</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="C16">
-        <v>0.97299999999999998</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
-        <v>7.0000000000000062E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000044E-3</v>
       </c>
       <c r="E16">
-        <v>0.98</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="F16">
-        <v>0.97299999999999998</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000062E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.0000000000000044E-3</v>
       </c>
       <c r="J16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="C17">
-        <v>0.99399999999999999</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.0000000000000053E-3</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F17">
-        <v>0.99399999999999999</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.0000000000000053E-3</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18">
-        <v>0.997</v>
+        <v>0.98</v>
       </c>
       <c r="C18">
-        <v>0.998</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
-        <v>1.0000000000000009E-3</v>
+        <f t="shared" si="5"/>
+        <v>7.0000000000000062E-3</v>
       </c>
       <c r="E18">
-        <v>0.997</v>
+        <v>0.98</v>
       </c>
       <c r="F18">
-        <v>0.998</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
-        <v>1.0000000000000009E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.0000000000000062E-3</v>
       </c>
       <c r="J18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>0.94499999999999995</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0.94499999999999995</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>6.0000000000000053E-3</v>
       </c>
       <c r="E19">
-        <v>0.94499999999999995</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>0.94499999999999995</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>6.0000000000000053E-3</v>
       </c>
       <c r="J19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20">
-        <v>0.98799999999999999</v>
+        <v>0.997</v>
       </c>
       <c r="C20">
-        <v>0.98699999999999999</v>
+        <v>0.998</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000009E-3</v>
       </c>
       <c r="E20">
-        <v>0.98799999999999999</v>
+        <v>0.997</v>
       </c>
       <c r="F20">
-        <v>0.98699999999999999</v>
+        <v>0.998</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
       <c r="J20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>0.997</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="C21">
-        <v>0.99299999999999999</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
-        <v>4.0000000000000036E-3</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0.997</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="F21">
-        <v>0.99299999999999999</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
-        <v>4.0000000000000036E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="J21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="C22">
-        <v>0.997</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
-        <v>3.0000000000000027E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F22">
-        <v>0.997</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
-        <v>3.0000000000000027E-3</v>
+        <f t="shared" si="3"/>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="J22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>0.997</v>
+      </c>
+      <c r="C23">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="5"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="E23">
+        <v>0.997</v>
+      </c>
+      <c r="F23">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.997</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="5"/>
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0.997</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>20</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>0.98899999999999999</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <v>0.997</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="3"/>
+      <c r="D25">
+        <f t="shared" si="5"/>
         <v>8.0000000000000071E-3</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <v>0.98899999999999999</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <v>0.997</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="1"/>
+      <c r="G25">
+        <f t="shared" si="3"/>
         <v>8.0000000000000071E-3</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="2"/>
+      <c r="J25">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Budget sonar results
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F46E9D1-53EE-4D80-AE02-296AB3B1D28D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2062499-D1D0-490D-928B-6345DF5ADC7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Data File Index</t>
   </si>
   <si>
-    <t>sonar</t>
-  </si>
-  <si>
     <t>KP Training Acc</t>
   </si>
   <si>
@@ -70,6 +67,12 @@
   </si>
   <si>
     <t>iris 113/37</t>
+  </si>
+  <si>
+    <t>sonar 157/51</t>
+  </si>
+  <si>
+    <t>sonar 116/92</t>
   </si>
 </sst>
 </file>
@@ -399,9 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -422,36 +423,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:D8" si="0">ABS(B2-C2)</f>
@@ -474,7 +475,7 @@
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" si="0"/>
@@ -497,15 +498,21 @@
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E4" s="2">
+        <v>0.54139999999999999</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.50980000000000003</v>
+      </c>
       <c r="G4" s="2">
         <f>ABS(E4-F4)</f>
-        <v>0</v>
+        <v>3.1599999999999961E-2</v>
       </c>
       <c r="J4" s="2">
         <f>ABS(H4-I4)</f>
@@ -514,15 +521,21 @@
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E5" s="2">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.51090000000000002</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" ref="G5:G25" si="3">ABS(E5-F5)</f>
-        <v>0</v>
+        <v>4.0799999999999947E-2</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ref="J5:J25" si="4">ABS(H5-I5)</f>

</xml_diff>

<commit_message>
Adding kernel perceptron real dataset results
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2062499-D1D0-490D-928B-6345DF5ADC7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C95205-92CE-4B83-A6ED-1C8B6F65930E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,7 +402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -454,6 +456,12 @@
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:D8" si="0">ABS(B2-C2)</f>
         <v>0</v>
@@ -477,6 +485,12 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
       <c r="D3" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -500,9 +514,15 @@
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B4" s="2">
+        <v>0.54139999999999999</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.50980000000000003</v>
+      </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.1599999999999961E-2</v>
       </c>
       <c r="E4" s="2">
         <v>0.54139999999999999</v>
@@ -523,9 +543,15 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B5" s="2">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.51090000000000002</v>
+      </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.0799999999999947E-2</v>
       </c>
       <c r="E5" s="2">
         <v>0.55169999999999997</v>

</xml_diff>

<commit_message>
Adding description results to spreadsheet with graph
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C95205-92CE-4B83-A6ED-1C8B6F65930E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECB31FB-F5F4-48E6-B83E-4C96D17E9FFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Data File Index</t>
   </si>
@@ -73,6 +73,33 @@
   </si>
   <si>
     <t>sonar 116/92</t>
+  </si>
+  <si>
+    <t>Avg KP synthetic training error:</t>
+  </si>
+  <si>
+    <t>Avg KP synthetic testing error</t>
+  </si>
+  <si>
+    <t>Avg KP synthetic Gen error</t>
+  </si>
+  <si>
+    <t>Avg KPB synthetic training error</t>
+  </si>
+  <si>
+    <t>Avg KPB synthetic testing error</t>
+  </si>
+  <si>
+    <t>Avg KPB synthetic Gen error</t>
+  </si>
+  <si>
+    <t>Avg KPD synthetic training error</t>
+  </si>
+  <si>
+    <t>Avg KPD synthetic testing error</t>
+  </si>
+  <si>
+    <t>Avg KPD synthetic Gen error</t>
   </si>
 </sst>
 </file>
@@ -135,6 +162,2331 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Synthetic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Generalization Error</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Kernel Perceptron</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$6:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0000000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0000000000000044E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0000000000000018E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0000000000000044E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000062E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.0000000000000036E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.0000000000000071E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7CC2-4BD3-AB66-ABF1143632C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Budget Kernel Perceptron</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$6:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0000000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0000000000000044E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0000000000000018E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0000000000000044E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000062E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.0000000000000036E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.0000000000000071E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-7CC2-4BD3-AB66-ABF1143632C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Description Kernel Perceptron</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$6:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$6:$J$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>9.000000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9999999999998943E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0000000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0000000000000062E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4000000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0000000000000018E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0000000000000018E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.0000000000000027E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0000000000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0000000000000044E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.0000000000000062E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0000000000000036E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.0000000000000053E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-7CC2-4BD3-AB66-ABF1143632C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="459323336"/>
+        <c:axId val="459322024"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$6:$B$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>0.96599999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.99399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.98899999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.96699999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.98399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.98799999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.996</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.97399999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.998</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.98199999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.98799999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.98</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.94499999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.98799999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.98899999999999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-7CC2-4BD3-AB66-ABF1143632C9}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$6:$C$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>0.96299999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.99299999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.97799999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.98899999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.98599999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.996</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.97299999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.999</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.97699999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.98199999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.97299999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.99399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.998</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.94499999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.98699999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.99299999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-7CC2-4BD3-AB66-ABF1143632C9}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$6:$E$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>0.96599999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.99399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.98899999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.96699999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.98399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.98799999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.996</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.97399999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.998</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.98199999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.98799999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.98</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.94499999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.98799999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.98899999999999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-7CC2-4BD3-AB66-ABF1143632C9}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$6:$F$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>0.96299999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.99299999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.97799999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.98899999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.98599999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.996</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.97299999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.999</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.97699999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.98199999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.97299999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.99399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.998</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.94499999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.98699999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.99299999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.997</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-7CC2-4BD3-AB66-ABF1143632C9}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="6"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$I$6:$I$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>0.97099999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.94199999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.99299999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.96099999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.97899999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.99</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.96199999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.97199999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.98199999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.94799999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.95599999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.95</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.97399999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.99399999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.98899999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.95799999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.99</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.92800000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.98</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.95499999999999996</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000007-7CC2-4BD3-AB66-ABF1143632C9}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="459323336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Synthetic</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Dataset Index</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459322024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="459322024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Generalization</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Error</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459323336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40BCC45E-961E-4730-B68B-6091AB1283D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,16 +2752,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
@@ -476,6 +2828,12 @@
         <f t="shared" ref="G2:G3" si="1">ABS(E2-F2)</f>
         <v>0</v>
       </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
       <c r="J2" s="2">
         <f t="shared" ref="J2:J3" si="2">ABS(H2-I2)</f>
         <v>0</v>
@@ -505,6 +2863,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
       <c r="J3" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -534,9 +2898,15 @@
         <f>ABS(E4-F4)</f>
         <v>3.1599999999999961E-2</v>
       </c>
+      <c r="H4" s="2">
+        <v>0.54139999999999999</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.50980000000000003</v>
+      </c>
       <c r="J4" s="2">
         <f>ABS(H4-I4)</f>
-        <v>0</v>
+        <v>3.1599999999999961E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -563,9 +2933,15 @@
         <f t="shared" ref="G5:G25" si="3">ABS(E5-F5)</f>
         <v>4.0799999999999947E-2</v>
       </c>
+      <c r="H5" s="2">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.51090000000000002</v>
+      </c>
       <c r="J5" s="2">
         <f t="shared" ref="J5:J25" si="4">ABS(H5-I5)</f>
-        <v>0</v>
+        <v>4.0799999999999947E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -592,9 +2968,15 @@
         <f t="shared" si="3"/>
         <v>3.0000000000000027E-3</v>
       </c>
+      <c r="H6">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="I6">
+        <v>0.97099999999999997</v>
+      </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9.000000000000008E-3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -621,9 +3003,15 @@
         <f t="shared" si="3"/>
         <v>3.0000000000000027E-3</v>
       </c>
+      <c r="H7">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="I7">
+        <v>0.94199999999999995</v>
+      </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.9999999999998943E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -650,9 +3038,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="H8">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="I8">
+        <v>0.99299999999999999</v>
+      </c>
       <c r="J8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -679,9 +3073,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-2</v>
       </c>
+      <c r="H9">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="I9">
+        <v>0.96099999999999997</v>
+      </c>
       <c r="J9">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -708,9 +3108,15 @@
         <f t="shared" si="3"/>
         <v>1.100000000000001E-2</v>
       </c>
+      <c r="H10">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="I10">
+        <v>0.97899999999999998</v>
+      </c>
       <c r="J10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.0000000000000009E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -737,9 +3143,15 @@
         <f t="shared" si="3"/>
         <v>5.0000000000000044E-3</v>
       </c>
+      <c r="H11">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="I11">
+        <v>0.99</v>
+      </c>
       <c r="J11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7.0000000000000062E-3</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -766,9 +3178,15 @@
         <f t="shared" si="3"/>
         <v>2.0000000000000018E-3</v>
       </c>
+      <c r="H12">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="I12">
+        <v>0.96199999999999997</v>
+      </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.100000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -795,9 +3213,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="H13">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="I13">
+        <v>0.97199999999999998</v>
+      </c>
       <c r="J13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.4000000000000012E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -824,9 +3248,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="H14">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="I14">
+        <v>0.98199999999999998</v>
+      </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.0000000000000053E-3</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -853,9 +3283,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="H15">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="I15">
+        <v>0.94799999999999995</v>
+      </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.0000000000000053E-3</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -882,9 +3318,15 @@
         <f t="shared" si="3"/>
         <v>5.0000000000000044E-3</v>
       </c>
+      <c r="H16">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="I16">
+        <v>0.95599999999999996</v>
+      </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.0000000000000018E-3</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -911,9 +3353,15 @@
         <f t="shared" si="3"/>
         <v>6.0000000000000053E-3</v>
       </c>
+      <c r="H17">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="I17">
+        <v>0.95</v>
+      </c>
       <c r="J17">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.0000000000000018E-3</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -940,9 +3388,15 @@
         <f t="shared" si="3"/>
         <v>7.0000000000000062E-3</v>
       </c>
+      <c r="H18">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="I18">
+        <v>0.97399999999999998</v>
+      </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.0000000000000027E-3</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -969,9 +3423,15 @@
         <f t="shared" si="3"/>
         <v>6.0000000000000053E-3</v>
       </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0.99399999999999999</v>
+      </c>
       <c r="J19">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.0000000000000053E-3</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -998,9 +3458,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="H20">
+        <v>0.99</v>
+      </c>
+      <c r="I20">
+        <v>0.98899999999999999</v>
+      </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1027,9 +3493,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="H21">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="I21">
+        <v>0.95799999999999996</v>
+      </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.0000000000000044E-3</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1056,9 +3528,15 @@
         <f t="shared" si="3"/>
         <v>1.0000000000000009E-3</v>
       </c>
+      <c r="H22">
+        <v>0.996</v>
+      </c>
+      <c r="I22">
+        <v>0.99</v>
+      </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.0000000000000053E-3</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1085,9 +3563,15 @@
         <f t="shared" si="3"/>
         <v>4.0000000000000036E-3</v>
       </c>
+      <c r="H23">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="I23">
+        <v>0.92800000000000005</v>
+      </c>
       <c r="J23">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7.0000000000000062E-3</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1114,9 +3598,15 @@
         <f t="shared" si="3"/>
         <v>3.0000000000000027E-3</v>
       </c>
+      <c r="H24">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I24">
+        <v>0.98</v>
+      </c>
       <c r="J24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.0000000000000036E-3</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1143,13 +3633,101 @@
         <f t="shared" si="3"/>
         <v>8.0000000000000071E-3</v>
       </c>
+      <c r="H25">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="I25">
+        <v>0.95499999999999996</v>
+      </c>
       <c r="J25">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.0000000000000053E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27">
+        <f>SUM(B6:B25)/20</f>
+        <v>0.98610000000000009</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <f>SUM(C6:C25)/20</f>
+        <v>0.9857999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <f>SUM(D6:D25)/20</f>
+        <v>3.9000000000000033E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31">
+        <f>SUM(E6:E25)/20</f>
+        <v>0.98610000000000009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32">
+        <f>SUM(F6:F25)/20</f>
+        <v>0.9857999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <f>SUM(G6:G25)/20</f>
+        <v>3.9000000000000033E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <f>SUM(H6:H25)/20</f>
+        <v>0.96914999999999973</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36">
+        <f>SUM(I6:I25)/20</f>
+        <v>0.96869999999999989</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37">
+        <f>SUM(J6:J25)/20</f>
+        <v>5.6499999999999996E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating spreadsheet with additional data and calculations
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECB31FB-F5F4-48E6-B83E-4C96D17E9FFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042F1F42-C94D-447C-B5D9-E80EF6468121}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Data File Index</t>
   </si>
@@ -100,6 +100,27 @@
   </si>
   <si>
     <t>Avg KPD synthetic Gen error</t>
+  </si>
+  <si>
+    <t>Standard deviation of KP</t>
+  </si>
+  <si>
+    <t>Standard deviation of KPB</t>
+  </si>
+  <si>
+    <t>Standard deviation of KPD</t>
+  </si>
+  <si>
+    <t>95% Confidence Interval KP</t>
+  </si>
+  <si>
+    <t>95% Confidence Interval KPB</t>
+  </si>
+  <si>
+    <t>95% Confidence Interval KPD</t>
+  </si>
+  <si>
+    <t>Synthetic</t>
   </si>
 </sst>
 </file>
@@ -728,7 +749,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -929,7 +949,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
@@ -1004,7 +1024,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$6:$C$25</c15:sqref>
@@ -1077,7 +1097,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-7CC2-4BD3-AB66-ABF1143632C9}"/>
                   </c:ext>
@@ -1100,7 +1120,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
@@ -1175,7 +1195,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$6:$E$25</c15:sqref>
@@ -1248,7 +1268,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-7CC2-4BD3-AB66-ABF1143632C9}"/>
                   </c:ext>
@@ -1271,7 +1291,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
@@ -1346,7 +1366,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$6:$F$25</c15:sqref>
@@ -1419,7 +1439,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-7CC2-4BD3-AB66-ABF1143632C9}"/>
                   </c:ext>
@@ -1444,7 +1464,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$6:$A$25</c15:sqref>
@@ -1519,7 +1539,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$6:$I$25</c15:sqref>
@@ -1592,7 +1612,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-7CC2-4BD3-AB66-ABF1143632C9}"/>
                   </c:ext>
@@ -2752,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3689,7 +3709,7 @@
         <v>0.9857999999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>19</v>
       </c>
@@ -3698,7 +3718,7 @@
         <v>3.9000000000000033E-3</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>20</v>
       </c>
@@ -3707,7 +3727,7 @@
         <v>0.96914999999999973</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>21</v>
       </c>
@@ -3716,13 +3736,85 @@
         <v>0.96869999999999989</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>22</v>
       </c>
       <c r="D37">
         <f>SUM(J6:J25)/20</f>
         <v>5.6499999999999996E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41">
+        <f>_xlfn.STDEV.S(D6:D25)</f>
+        <v>3.2751054623437253E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42">
+        <f>_xlfn.STDEV.S(G6:G25)</f>
+        <v>3.2751054623437253E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43">
+        <f>_xlfn.STDEV.S(J6:J25)</f>
+        <v>3.513507768897813E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, D41, 20)</f>
+        <v>1.4353518802548806E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46">
+        <f>_xlfn.CONFIDENCE.NORM(0.05,D42,20)</f>
+        <v>1.4353518802548806E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, D43,20)</f>
+        <v>1.5398343779649333E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding sonar timing results
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF78BEC8-AFDA-409D-B74A-472EB3296EE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4C1240-A9DC-4E8C-968E-049402E0CAC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2251,6 +2251,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
               <c:f>Timing!$A$2:$A$21</c:f>
@@ -2447,6 +2464,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
               <c:f>Timing!$A$2:$A$21</c:f>
@@ -3274,6 +3308,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
               <c:f>Timing!$A$2:$A$21</c:f>
@@ -3771,6 +3822,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="411439712"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4026,6 +4078,24 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Timing!$A$22:$A$23</c:f>
@@ -4135,6 +4205,24 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Timing!$A$22:$A$23</c:f>
@@ -4246,6 +4334,24 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Timing!$A$22:$A$23</c:f>
@@ -4465,7 +4571,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4487,7 +4593,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$A$22:$A$23</c15:sqref>
@@ -4507,7 +4613,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$E$22:$E$23</c15:sqref>
@@ -4520,7 +4626,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-3EF8-4DCB-8A87-ACC09B9D146B}"/>
                   </c:ext>
@@ -4579,7 +4685,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4601,7 +4707,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$A$22:$A$23</c15:sqref>
@@ -4621,7 +4727,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$F$22:$F$23</c15:sqref>
@@ -4634,7 +4740,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-3EF8-4DCB-8A87-ACC09B9D146B}"/>
                   </c:ext>
@@ -4693,7 +4799,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4715,7 +4821,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$A$22:$A$23</c15:sqref>
@@ -4735,7 +4841,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$G$22:$G$23</c15:sqref>
@@ -4748,7 +4854,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-3EF8-4DCB-8A87-ACC09B9D146B}"/>
                   </c:ext>
@@ -4809,7 +4915,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4831,7 +4937,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$A$22:$A$23</c15:sqref>
@@ -4851,7 +4957,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$H$22:$H$23</c15:sqref>
@@ -4864,7 +4970,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-3EF8-4DCB-8A87-ACC09B9D146B}"/>
                   </c:ext>
@@ -4925,7 +5031,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -4947,7 +5053,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$A$22:$A$23</c15:sqref>
@@ -4967,7 +5073,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Timing!$I$22:$I$23</c15:sqref>
@@ -4980,7 +5086,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-3EF8-4DCB-8A87-ACC09B9D146B}"/>
                   </c:ext>
@@ -6963,16 +7069,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7265,8 +7371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8497,8 +8603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAB718F-DF94-4DDA-BA48-1B1D5687EE31}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8904,10 +9010,34 @@
       <c r="A24" t="s">
         <v>51</v>
       </c>
+      <c r="C24">
+        <f>(83.226+78.271+78.045+77.998+77.599)/5</f>
+        <v>79.027799999999999</v>
+      </c>
+      <c r="D24">
+        <f>(68.773+65.812+65.477+65.397+65.385)/5</f>
+        <v>66.168800000000005</v>
+      </c>
+      <c r="J24">
+        <f>(1044.636+1046.609+1047.802+1046.586+1043.563)/5</f>
+        <v>1045.8391999999999</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
+      </c>
+      <c r="C25">
+        <f>(146.986+136.707+136.165+136.848+136.622)/5</f>
+        <v>138.66559999999998</v>
+      </c>
+      <c r="D25">
+        <f>(127.937+120.138+120.142+120.378+119.713)/5</f>
+        <v>121.66159999999999</v>
+      </c>
+      <c r="J25">
+        <f>(2120.556+2123.456+2126.547+2127.52+2109.276)/5</f>
+        <v>2121.4710000000005</v>
       </c>
     </row>
   </sheetData>
@@ -8921,7 +9051,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding generalization error calculations to spreadsheet
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4C1240-A9DC-4E8C-968E-049402E0CAC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62D2D8F-B0E5-4E5F-BCD8-87D85FE6C360}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GenError" sheetId="1" r:id="rId1"/>
-    <sheet name="Timing" sheetId="3" r:id="rId2"/>
-    <sheet name="GenErrorCalc" sheetId="2" r:id="rId3"/>
+    <sheet name="GenErrorCalc" sheetId="2" r:id="rId2"/>
+    <sheet name="Timing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="228">
   <si>
     <t>Data File Index</t>
   </si>
@@ -134,21 +134,6 @@
     <t>eps</t>
   </si>
   <si>
-    <t>KP Training Set Size</t>
-  </si>
-  <si>
-    <t>KPB Training Set Size</t>
-  </si>
-  <si>
-    <t>KPD Training Set Size</t>
-  </si>
-  <si>
-    <t>KPB Support Set Size</t>
-  </si>
-  <si>
-    <t>KPD Support Set Size</t>
-  </si>
-  <si>
     <t>KP</t>
   </si>
   <si>
@@ -158,9 +143,6 @@
     <t>KPD</t>
   </si>
   <si>
-    <t>Dimensionality</t>
-  </si>
-  <si>
     <t>sonar 157/51 10k norm</t>
   </si>
   <si>
@@ -207,12 +189,543 @@
   </si>
   <si>
     <t>Description Kernel Perceptron</t>
+  </si>
+  <si>
+    <t>1000 Training Examples</t>
+  </si>
+  <si>
+    <t>100 Budget/Mistakes</t>
+  </si>
+  <si>
+    <t>6.90947E+38531</t>
+  </si>
+  <si>
+    <t>1.42415E+38523</t>
+  </si>
+  <si>
+    <t>1.24706E+38497</t>
+  </si>
+  <si>
+    <t>4.63915E+38453</t>
+  </si>
+  <si>
+    <t>7.33180E+38392</t>
+  </si>
+  <si>
+    <t>4.92271E+38314</t>
+  </si>
+  <si>
+    <t>1.40416E+38219</t>
+  </si>
+  <si>
+    <t>1.70158E+38106</t>
+  </si>
+  <si>
+    <t>8.76008E+37975</t>
+  </si>
+  <si>
+    <t>1.91595E+37828</t>
+  </si>
+  <si>
+    <t>1.78025E+37663</t>
+  </si>
+  <si>
+    <t>KP: ((2^64)/e^(eps^2))^2000</t>
+  </si>
+  <si>
+    <t>n = 3</t>
+  </si>
+  <si>
+    <t>1.93617E+3883</t>
+  </si>
+  <si>
+    <t>3.99075E+3874</t>
+  </si>
+  <si>
+    <t>3.49450E+3848</t>
+  </si>
+  <si>
+    <t>1.29998E+3805</t>
+  </si>
+  <si>
+    <t>2.05452E+3744</t>
+  </si>
+  <si>
+    <t>1.37944E+3666</t>
+  </si>
+  <si>
+    <t>3.93475E+3570</t>
+  </si>
+  <si>
+    <t>4.76817E+3457</t>
+  </si>
+  <si>
+    <t>2.45475E+3327</t>
+  </si>
+  <si>
+    <t>5.36888E+3179</t>
+  </si>
+  <si>
+    <t>4.98862E+3014</t>
+  </si>
+  <si>
+    <t>KPB: ((2^645)/e^(100*(eps^2)))^20</t>
+  </si>
+  <si>
+    <t>4.20647E+2929</t>
+  </si>
+  <si>
+    <t>8.67018E+2920</t>
+  </si>
+  <si>
+    <t>7.59205E+2894</t>
+  </si>
+  <si>
+    <t>2.82430E+2851</t>
+  </si>
+  <si>
+    <t>4.46358E+2790</t>
+  </si>
+  <si>
+    <t>2.99693E+2712</t>
+  </si>
+  <si>
+    <t>8.54852E+2616</t>
+  </si>
+  <si>
+    <t>1.03592E+2504</t>
+  </si>
+  <si>
+    <t>5.33312E+2373</t>
+  </si>
+  <si>
+    <t>1.16643E+2226</t>
+  </si>
+  <si>
+    <t>1.08381E+2061</t>
+  </si>
+  <si>
+    <t>KPD: (2^9732)/e^(2000*(eps^2))</t>
+  </si>
+  <si>
+    <t>77 Training Examples</t>
+  </si>
+  <si>
+    <t>7 Budget/Mistakes</t>
+  </si>
+  <si>
+    <t>n = 4</t>
+  </si>
+  <si>
+    <t>3.08721E+3036</t>
+  </si>
+  <si>
+    <t>6.61840E+3035</t>
+  </si>
+  <si>
+    <t>6.52097E+3033</t>
+  </si>
+  <si>
+    <t>2.95287E+3030</t>
+  </si>
+  <si>
+    <t>6.14540E+3025</t>
+  </si>
+  <si>
+    <t>5.87799E+3019</t>
+  </si>
+  <si>
+    <t>2.58393E+3012</t>
+  </si>
+  <si>
+    <t>5.22041E+3003</t>
+  </si>
+  <si>
+    <t>4.84732E+2993</t>
+  </si>
+  <si>
+    <t>2.06858E+2982</t>
+  </si>
+  <si>
+    <t>4.05710E+2969</t>
+  </si>
+  <si>
+    <t>KP: ((2^131)/e^(2*(eps^2)))^77</t>
+  </si>
+  <si>
+    <t>Synthetic Datasets</t>
+  </si>
+  <si>
+    <t>Iris Dataset 50/50 Split</t>
+  </si>
+  <si>
+    <t>KPB: ((2^129)/e^(22*(eps^2)))^7</t>
+  </si>
+  <si>
+    <t>KPD: (2^711)/e^(154*(eps^2))</t>
+  </si>
+  <si>
+    <t>Iris Dataset 75/25 Split</t>
+  </si>
+  <si>
+    <t>116 Training Examples</t>
+  </si>
+  <si>
+    <t>11 Budget/Mistakes</t>
+  </si>
+  <si>
+    <t>1.33083E+533</t>
+  </si>
+  <si>
+    <t>6.23051E+436</t>
+  </si>
+  <si>
+    <t>Sonar Dataset 50/50 Split</t>
+  </si>
+  <si>
+    <t>113 Training Examples</t>
+  </si>
+  <si>
+    <t>n = 60</t>
+  </si>
+  <si>
+    <t>4.19104E+5442</t>
+  </si>
+  <si>
+    <t>4.37337E+5441</t>
+  </si>
+  <si>
+    <t>4.96935E+5438</t>
+  </si>
+  <si>
+    <t>6.14854E+5433</t>
+  </si>
+  <si>
+    <t>8.28387E+5426</t>
+  </si>
+  <si>
+    <t>1.21530E+5418</t>
+  </si>
+  <si>
+    <t>1.94143E+5407</t>
+  </si>
+  <si>
+    <t>3.37715E+5394</t>
+  </si>
+  <si>
+    <t>6.39687E+5379</t>
+  </si>
+  <si>
+    <t>1.31939E+5363</t>
+  </si>
+  <si>
+    <t>2.96325E+5344</t>
+  </si>
+  <si>
+    <t>KP: ((2^80)/e^(eps^2))^226</t>
+  </si>
+  <si>
+    <t>1.38873E+532</t>
+  </si>
+  <si>
+    <t>1.57798E+529</t>
+  </si>
+  <si>
+    <t>1.95242E+524</t>
+  </si>
+  <si>
+    <t>2.63047E+517</t>
+  </si>
+  <si>
+    <t>3.85908E+508</t>
+  </si>
+  <si>
+    <t>6.16486E+497</t>
+  </si>
+  <si>
+    <t>1.07239E+485</t>
+  </si>
+  <si>
+    <t>2.03127E+470</t>
+  </si>
+  <si>
+    <t>4.18962E+453</t>
+  </si>
+  <si>
+    <t>9.40956E+434</t>
+  </si>
+  <si>
+    <t>KPB: (2^1771)/e^(226*(eps^2))</t>
+  </si>
+  <si>
+    <t>6.50157E+435</t>
+  </si>
+  <si>
+    <t>7.38757E+432</t>
+  </si>
+  <si>
+    <t>9.14058E+427</t>
+  </si>
+  <si>
+    <t>1.23150E+421</t>
+  </si>
+  <si>
+    <t>1.80670E+412</t>
+  </si>
+  <si>
+    <t>2.88619E+401</t>
+  </si>
+  <si>
+    <t>5.02057E+388</t>
+  </si>
+  <si>
+    <t>9.50977E+373</t>
+  </si>
+  <si>
+    <t>1.96144E+357</t>
+  </si>
+  <si>
+    <t>4.40525E+338</t>
+  </si>
+  <si>
+    <t>6.66773E+68162</t>
+  </si>
+  <si>
+    <t>6.55262E+68161</t>
+  </si>
+  <si>
+    <t>6.21907E+68158</t>
+  </si>
+  <si>
+    <t>5.70045E+68153</t>
+  </si>
+  <si>
+    <t>5.04623E+68146</t>
+  </si>
+  <si>
+    <t>4.31418E+68137</t>
+  </si>
+  <si>
+    <t>3.56207E+68126</t>
+  </si>
+  <si>
+    <t>2.84041E+68113</t>
+  </si>
+  <si>
+    <t>2.18743E+68098</t>
+  </si>
+  <si>
+    <t>1.62689E+68081</t>
+  </si>
+  <si>
+    <t>Would not compute</t>
+  </si>
+  <si>
+    <t>KP: ((2^976)/e^(eps^2))^232</t>
+  </si>
+  <si>
+    <t>1.06512E+6467</t>
+  </si>
+  <si>
+    <t>1.04673E+6466</t>
+  </si>
+  <si>
+    <t>9.93446E+6462</t>
+  </si>
+  <si>
+    <t>9.10601E+6457</t>
+  </si>
+  <si>
+    <t>8.06094E+6450</t>
+  </si>
+  <si>
+    <t>6.89155E+6441</t>
+  </si>
+  <si>
+    <t>5.69012E+6430</t>
+  </si>
+  <si>
+    <t>4.53733E+6417</t>
+  </si>
+  <si>
+    <t>3.49424E+6402</t>
+  </si>
+  <si>
+    <t>2.59883E+6385</t>
+  </si>
+  <si>
+    <t>1.86671E+6366</t>
+  </si>
+  <si>
+    <t>KPB: (2^21483)/e^(232*(eps^2))</t>
+  </si>
+  <si>
+    <t>4.98653E+6370</t>
+  </si>
+  <si>
+    <t>4.90044E+6369</t>
+  </si>
+  <si>
+    <t>4.65099E+6366</t>
+  </si>
+  <si>
+    <t>4.26314E+6361</t>
+  </si>
+  <si>
+    <t>3.77387E+6354</t>
+  </si>
+  <si>
+    <t>3.22640E+6345</t>
+  </si>
+  <si>
+    <t>2.66393E+6334</t>
+  </si>
+  <si>
+    <t>2.12423E+6321</t>
+  </si>
+  <si>
+    <t>1.63589E+6306</t>
+  </si>
+  <si>
+    <t>1.21669E+6289</t>
+  </si>
+  <si>
+    <t>8.73934E+6269</t>
+  </si>
+  <si>
+    <t>KPD: (2^21163)/e^(232*(eps^2))</t>
+  </si>
+  <si>
+    <t>Sonar Dataset 75/25 Split</t>
+  </si>
+  <si>
+    <t>157 Training Examples</t>
+  </si>
+  <si>
+    <t>15 Budget/Mistakes</t>
+  </si>
+  <si>
+    <t>7.18772E+92254</t>
+  </si>
+  <si>
+    <t>3.11105E+92253</t>
+  </si>
+  <si>
+    <t>2.52262E+92249</t>
+  </si>
+  <si>
+    <t>3.83203E+92242</t>
+  </si>
+  <si>
+    <t>1.09053E+92233</t>
+  </si>
+  <si>
+    <t>5.81399E+92220</t>
+  </si>
+  <si>
+    <t>5.80688E+92205</t>
+  </si>
+  <si>
+    <t>1.08653E+92188</t>
+  </si>
+  <si>
+    <t>3.80866E+92167</t>
+  </si>
+  <si>
+    <t>2.50111E+92144</t>
+  </si>
+  <si>
+    <t>KP: ((2^976)/e^(eps^2))^314</t>
+  </si>
+  <si>
+    <t>4.71762E+8818</t>
+  </si>
+  <si>
+    <t>2.04192E+8817</t>
+  </si>
+  <si>
+    <t>1.65571E+8813</t>
+  </si>
+  <si>
+    <t>2.51513E+8806</t>
+  </si>
+  <si>
+    <t>7.15761E+8796</t>
+  </si>
+  <si>
+    <t>3.81598E+8784</t>
+  </si>
+  <si>
+    <t>3.81131E+8769</t>
+  </si>
+  <si>
+    <t>7.13139E+8751</t>
+  </si>
+  <si>
+    <t>2.49979E+8731</t>
+  </si>
+  <si>
+    <t>1.64159E+8708</t>
+  </si>
+  <si>
+    <t>2.01955E+8682</t>
+  </si>
+  <si>
+    <t>KPB: (2^29295)/e^(314*(eps^2))</t>
+  </si>
+  <si>
+    <t>KPD: (2^28847)/e^(314*(eps^2))</t>
+  </si>
+  <si>
+    <t>6.49060E+8683</t>
+  </si>
+  <si>
+    <t>2.80931E+8682</t>
+  </si>
+  <si>
+    <t>2.27796E+8678</t>
+  </si>
+  <si>
+    <t>3.46037E+8671</t>
+  </si>
+  <si>
+    <t>9.84759E+8661</t>
+  </si>
+  <si>
+    <t>5.25011E+8649</t>
+  </si>
+  <si>
+    <t>5.24369E+8634</t>
+  </si>
+  <si>
+    <t>9.81151E+8616</t>
+  </si>
+  <si>
+    <t>3.43927E+8596</t>
+  </si>
+  <si>
+    <t>2.25853E+8573</t>
+  </si>
+  <si>
+    <t>2.77855E+8547</t>
+  </si>
+  <si>
+    <t>1000 training examples</t>
+  </si>
+  <si>
+    <t>2 support vectors</t>
+  </si>
+  <si>
+    <t>2 mistakes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,10 +763,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7371,7 +7887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -8334,12 +8850,12 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>0.84079999999999999</v>
@@ -8354,7 +8870,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -8369,10 +8885,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E33">
         <v>0.85350000000000004</v>
@@ -8387,10 +8903,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -8405,10 +8921,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E35">
         <v>0.54139999999999999</v>
@@ -8423,10 +8939,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E36">
         <v>0.55169999999999997</v>
@@ -8600,10 +9116,1251 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D4E763-7B26-4572-B2E3-B397149B68CA}">
+  <dimension ref="A1:F91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="4">
+        <v>6.7621700000000005E+271</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.07728E+214</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.44968E+271</v>
+      </c>
+      <c r="E16" s="4">
+        <v>2.3094800000000001E+213</v>
+      </c>
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.42834E+269</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2.27548E+211</v>
+      </c>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.3</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="4">
+        <v>6.4679200000000003E+265</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.0304E+208</v>
+      </c>
+      <c r="F18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.3460800000000001E+261</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2.1444299999999999E+203</v>
+      </c>
+      <c r="F19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1.2875000000000001E+255</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2.0511100000000001E+197</v>
+      </c>
+      <c r="F20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.6</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5.6597900000000001E+247</v>
+      </c>
+      <c r="E21" s="4">
+        <v>9.0165599999999994E+189</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.7</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1.14347E+239</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1.8216500000000001E+181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.8</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1.06175E+229</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1.6914600000000001E+171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.9</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4.5309799999999996E+217</v>
+      </c>
+      <c r="E24" s="4">
+        <v>7.21827E+159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="4">
+        <v>8.8865999999999997E+204</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1.41572E+147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.2</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.3</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.4</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.6</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.7</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.8</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.9</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.1</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.2</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.3</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.4</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0.5</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0.6</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0.7</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0.8</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0.9</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0.1</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F55" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0.2</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F56" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0.3</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F57" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0.4</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F58" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0.5</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F59" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0.6</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F60" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0.7</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.8</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0.9</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>0</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67">
+        <f>POWER(2, 2*32+(1+3*32)*2)/EXP(2*1000*A67^2)</f>
+        <v>4.6316835694926478E+77</v>
+      </c>
+      <c r="F67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68">
+        <f t="shared" ref="D68:D77" si="0">POWER(2, 2*32+(1+3*32)*2)/EXP(2*1000*A68^2)</f>
+        <v>9.5466113672488865E+68</v>
+      </c>
+      <c r="F68" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69">
+        <f t="shared" si="0"/>
+        <v>8.3595005184594924E+42</v>
+      </c>
+      <c r="F69" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1">
+        <f t="shared" si="0"/>
+        <v>0.31097977050255327</v>
+      </c>
+      <c r="F70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71">
+        <f t="shared" si="0"/>
+        <v>4.9147866764149157E-62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72">
+        <f t="shared" si="0"/>
+        <v>3.2998783482698575E-140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0.6</v>
+      </c>
+      <c r="D73" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0.7</v>
+      </c>
+      <c r="D74" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0.8</v>
+      </c>
+      <c r="D75" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0.9</v>
+      </c>
+      <c r="D76" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="4"/>
+      <c r="E79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>0</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="E80">
+        <f>POWER(2, 32+(1+3*32)*2)/EXP(2000*A80^2)</f>
+        <v>1.0783978666860256E+68</v>
+      </c>
+      <c r="F80" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="E81">
+        <f t="shared" ref="E81:E91" si="1">POWER(2, 32+(1+3*32)*2)/EXP(2000*A81^2)</f>
+        <v>2.2227436693499066E+59</v>
+      </c>
+      <c r="F81" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="E82">
+        <f t="shared" si="1"/>
+        <v>1.9463478863377805E+33</v>
+      </c>
+      <c r="F82" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1">
+        <f t="shared" si="1"/>
+        <v>9.101443183444155E-2</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E84" s="2">
+        <f t="shared" si="1"/>
+        <v>7.2405620129442137E-11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="E85">
+        <f t="shared" si="1"/>
+        <v>1.1443129452911475E-71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="E86">
+        <f t="shared" si="1"/>
+        <v>7.683127998071391E-150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>0.6</v>
+      </c>
+      <c r="E87" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0.7</v>
+      </c>
+      <c r="E88" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>0.8</v>
+      </c>
+      <c r="E89" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>0.9</v>
+      </c>
+      <c r="E90" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1</v>
+      </c>
+      <c r="E91" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAB718F-DF94-4DDA-BA48-1B1D5687EE31}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -8617,19 +10374,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -8974,7 +10731,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <f>(0.013+0.003+0.003+0.003+0.003)/5</f>
@@ -8991,7 +10748,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C23">
         <f>(0.017+0.006+0.005+0.005+0.005)/5</f>
@@ -9008,7 +10765,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C24">
         <f>(83.226+78.271+78.045+77.998+77.599)/5</f>
@@ -9025,7 +10782,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C25">
         <f>(146.986+136.707+136.165+136.848+136.622)/5</f>
@@ -9044,273 +10801,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D4E763-7B26-4572-B2E3-B397149B68CA}">
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A2^2*E14)</f>
-        <v>3.4028236692093846E+38</v>
-      </c>
-      <c r="D2">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A2^2)</f>
-        <v>6.8056473384187693E+38</v>
-      </c>
-      <c r="E2">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A2^2)</f>
-        <v>6.8056473384187693E+38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.1</v>
-      </c>
-      <c r="C3">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A3^2*E14)</f>
-        <v>3.3354432460558638E+38</v>
-      </c>
-      <c r="D3">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A3^2)</f>
-        <v>1.4027484664621126E+30</v>
-      </c>
-      <c r="E3">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A3^2)</f>
-        <v>1.4027484664621126E+30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.2</v>
-      </c>
-      <c r="C4">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A4^2*E14)</f>
-        <v>3.1412021529185332E+38</v>
-      </c>
-      <c r="D4">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A4^2)</f>
-        <v>12283.182043931398</v>
-      </c>
-      <c r="E4">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A4^2)</f>
-        <v>12283.182043931398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0.3</v>
-      </c>
-      <c r="C5">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A5^2*E14)</f>
-        <v>2.842277245575803E+38</v>
-      </c>
-      <c r="D5">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A5^2)</f>
-        <v>4.5694370430720351E-40</v>
-      </c>
-      <c r="E5">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A5^2)</f>
-        <v>4.5694370430720351E-40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0.4</v>
-      </c>
-      <c r="C6">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A6^2*E14)</f>
-        <v>2.4709571307279581E+38</v>
-      </c>
-      <c r="D6">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A6^2)</f>
-        <v>7.2216299670279742E-101</v>
-      </c>
-      <c r="E6">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A6^2)</f>
-        <v>7.2216299670279742E-101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0.5</v>
-      </c>
-      <c r="C7">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A7^2*E14)</f>
-        <v>2.063916884971332E+38</v>
-      </c>
-      <c r="D7">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A7^2)</f>
-        <v>4.8487354459899989E-179</v>
-      </c>
-      <c r="E7">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A7^2)</f>
-        <v>4.8487354459899989E-179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.6</v>
-      </c>
-      <c r="C8">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A8^2*E14)</f>
-        <v>1.6563320976216564E+38</v>
-      </c>
-      <c r="D8">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A8^2)</f>
-        <v>1.3830646151531151E-274</v>
-      </c>
-      <c r="E8">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A8^2)</f>
-        <v>1.3830646151531151E-274</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0.7</v>
-      </c>
-      <c r="C9">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A9^2*E14)</f>
-        <v>1.2771174904885256E+38</v>
-      </c>
-      <c r="D9">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A9^2)</f>
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A9^2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0.8</v>
-      </c>
-      <c r="C10">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A10^2*E14)</f>
-        <v>9.4611190690520998E+37</v>
-      </c>
-      <c r="D10">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A10^2)</f>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A10^2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0.9</v>
-      </c>
-      <c r="C11">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A11^2*E14)</f>
-        <v>6.734143773474695E+37</v>
-      </c>
-      <c r="D11">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A11^2)</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A11^2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <f>POWER(2,(E14*E21*32 +32*E14))*EXP(-2*A12^2*E14)</f>
-        <v>4.6052210507670176E+37</v>
-      </c>
-      <c r="D12">
-        <f>POWER(2,(32*E18+(1+E21*32)*E18))*EXP(-2*E15*A12^2)</f>
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f>POWER(2, (32+(1+E21*32)*E19))*EXP(-2*E16*A12^2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding results of running KPB and KPD with inputs to match generalization error calculations
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62D2D8F-B0E5-4E5F-BCD8-87D85FE6C360}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF30570-F4FC-482C-B172-40B4FC7871CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GenError" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="235">
   <si>
     <t>Data File Index</t>
   </si>
@@ -717,6 +717,27 @@
   </si>
   <si>
     <t>2 mistakes</t>
+  </si>
+  <si>
+    <t>KPB Training 2</t>
+  </si>
+  <si>
+    <t>KPB Test</t>
+  </si>
+  <si>
+    <t>KPD Training 2</t>
+  </si>
+  <si>
+    <t>KPD Test</t>
+  </si>
+  <si>
+    <t>KPD Generalization &lt; .09</t>
+  </si>
+  <si>
+    <t>KPB Generalization &lt; .09</t>
+  </si>
+  <si>
+    <t>Synthetic Gen Err Run</t>
   </si>
 </sst>
 </file>
@@ -7885,10 +7906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9036,7 +9057,7 @@
         <v>5.6499999999999996E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -9048,7 +9069,7 @@
         <v>3.2751054623437253E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -9060,7 +9081,7 @@
         <v>3.2751054623437253E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -9072,7 +9093,7 @@
         <v>3.513507768897813E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -9084,7 +9105,7 @@
         <v>1.4353518802548806E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -9096,7 +9117,7 @@
         <v>1.4353518802548806E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -9106,6 +9127,600 @@
       <c r="D58">
         <f>_xlfn.CONFIDENCE.NORM(0.05, D54,20)</f>
         <v>1.5398343779649333E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>228</v>
+      </c>
+      <c r="F60" t="s">
+        <v>229</v>
+      </c>
+      <c r="G60" t="s">
+        <v>233</v>
+      </c>
+      <c r="H60" t="s">
+        <v>230</v>
+      </c>
+      <c r="I60" t="s">
+        <v>231</v>
+      </c>
+      <c r="J60" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="F61">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G61">
+        <f>ABS(E61-F61)</f>
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="H61">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="I61">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="J61">
+        <f>ABS(H61-I61)</f>
+        <v>2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F62">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="G62">
+        <f t="shared" ref="G62:G80" si="7">ABS(E62-F62)</f>
+        <v>2.6999999999999913E-2</v>
+      </c>
+      <c r="H62">
+        <v>0.81</v>
+      </c>
+      <c r="I62">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="J62">
+        <f t="shared" ref="J62:J80" si="8">ABS(H62-I62)</f>
+        <v>1.7000000000000015E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F63">
+        <v>0.82</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="7"/>
+        <v>1.19999999999999E-2</v>
+      </c>
+      <c r="H63">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="I63">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="8"/>
+        <v>9.000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="F64">
+        <v>0.753</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="7"/>
+        <v>2.7000000000000024E-2</v>
+      </c>
+      <c r="H64">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="I64">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="8"/>
+        <v>1.2000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="E65">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="F65">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="7"/>
+        <v>1.9000000000000017E-2</v>
+      </c>
+      <c r="H65">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="I65">
+        <v>0.876</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="8"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="F66">
+        <v>0.75</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="7"/>
+        <v>1.7000000000000015E-2</v>
+      </c>
+      <c r="H66">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="I66">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="8"/>
+        <v>1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>7</v>
+      </c>
+      <c r="E67">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="F67">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="7"/>
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="H67">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="I67">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="8"/>
+        <v>4.2999999999999927E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>8</v>
+      </c>
+      <c r="E68">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="F68">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="7"/>
+        <v>1.2000000000000011E-2</v>
+      </c>
+      <c r="H68">
+        <v>0.71</v>
+      </c>
+      <c r="I68">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="8"/>
+        <v>3.0000000000000027E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>9</v>
+      </c>
+      <c r="E69">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="F69">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="7"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+      <c r="H69">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="I69">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="8"/>
+        <v>1.4999999999999902E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="E70">
+        <v>0.8</v>
+      </c>
+      <c r="F70">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="7"/>
+        <v>2.1000000000000019E-2</v>
+      </c>
+      <c r="H70">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="I70">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="8"/>
+        <v>4.599999999999993E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>11</v>
+      </c>
+      <c r="E71">
+        <v>0.59</v>
+      </c>
+      <c r="F71">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="7"/>
+        <v>2.1000000000000019E-2</v>
+      </c>
+      <c r="H71">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="I71">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="8"/>
+        <v>6.0000000000000053E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>12</v>
+      </c>
+      <c r="E72">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="F72">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="H72">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="I72">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>13</v>
+      </c>
+      <c r="E73">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="F73">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="7"/>
+        <v>1.2000000000000011E-2</v>
+      </c>
+      <c r="H73">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="I73">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="8"/>
+        <v>2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>14</v>
+      </c>
+      <c r="E74">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F74">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="7"/>
+        <v>1.0000000000000009E-3</v>
+      </c>
+      <c r="H74">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="I74">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="8"/>
+        <v>1.100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>15</v>
+      </c>
+      <c r="E75">
+        <v>0.51</v>
+      </c>
+      <c r="F75">
+        <v>0.54</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="7"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="H75">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="I75">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="8"/>
+        <v>2.4999999999999911E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>16</v>
+      </c>
+      <c r="E76">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="F76">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="7"/>
+        <v>5.0000000000000044E-3</v>
+      </c>
+      <c r="H76">
+        <v>0.747</v>
+      </c>
+      <c r="I76">
+        <v>0.751</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="8"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>17</v>
+      </c>
+      <c r="E77">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="F77">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="7"/>
+        <v>5.699999999999994E-2</v>
+      </c>
+      <c r="H77">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="I77">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="8"/>
+        <v>4.7999999999999932E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>18</v>
+      </c>
+      <c r="E78">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="F78">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="7"/>
+        <v>1.3000000000000012E-2</v>
+      </c>
+      <c r="H78">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="I78">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="8"/>
+        <v>4.4999999999999929E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>19</v>
+      </c>
+      <c r="E79">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="F79">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="7"/>
+        <v>3.3000000000000029E-2</v>
+      </c>
+      <c r="H79">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="I79">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="8"/>
+        <v>7.0000000000000062E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>20</v>
+      </c>
+      <c r="E80">
+        <v>0.89</v>
+      </c>
+      <c r="F80">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="7"/>
+        <v>6.0000000000000053E-3</v>
+      </c>
+      <c r="H80">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="I80">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <f>AVERAGE(E61:E80)</f>
+        <v>0.76890000000000014</v>
+      </c>
+      <c r="F81">
+        <f t="shared" ref="F81:J81" si="9">AVERAGE(F61:F80)</f>
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="9"/>
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="9"/>
+        <v>0.78625000000000012</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="9"/>
+        <v>0.78110000000000002</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="9"/>
+        <v>1.8049999999999983E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>234</v>
+      </c>
+      <c r="B82" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82">
+        <f>_xlfn.STDEV.S(G61:G80)</f>
+        <v>1.3222389305544141E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>234</v>
+      </c>
+      <c r="B83" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83">
+        <f>_xlfn.STDEV.S(J61:J80)</f>
+        <v>1.5988400400553528E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>234</v>
+      </c>
+      <c r="B85" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85">
+        <f>_xlfn.CONFIDENCE.NORM(0.05,D82,20)</f>
+        <v>5.7948611332940842E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>234</v>
+      </c>
+      <c r="B86" t="s">
+        <v>28</v>
+      </c>
+      <c r="D86">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, D83,20)</f>
+        <v>7.0070966694244039E-3</v>
       </c>
     </row>
   </sheetData>
@@ -9117,10 +9732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D4E763-7B26-4572-B2E3-B397149B68CA}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10104,7 +10719,7 @@
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68">
-        <f t="shared" ref="D68:D77" si="0">POWER(2, 2*32+(1+3*32)*2)/EXP(2*1000*A68^2)</f>
+        <f t="shared" ref="D68:D78" si="0">POWER(2, 2*32+(1+3*32)*2)/EXP(2*1000*A68^2)</f>
         <v>9.5466113672488865E+68</v>
       </c>
       <c r="F68" t="s">
@@ -10126,12 +10741,12 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70" s="2">
         <v>0.3</v>
       </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70">
         <f t="shared" si="0"/>
         <v>0.31097977050255327</v>
       </c>
@@ -10140,39 +10755,41 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71">
+      <c r="A71" s="1">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1">
         <f t="shared" si="0"/>
-        <v>4.9147866764149157E-62</v>
+        <v>9.3478163489151653E-2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72">
         <f t="shared" si="0"/>
+        <v>4.9147866764149157E-62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73">
+        <f t="shared" si="0"/>
         <v>3.2998783482698575E-140</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>0.6</v>
-      </c>
-      <c r="D73" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D74" t="e">
         <f t="shared" si="0"/>
@@ -10181,7 +10798,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D75" t="e">
         <f t="shared" si="0"/>
@@ -10190,7 +10807,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D76" t="e">
         <f t="shared" si="0"/>
@@ -10199,124 +10816,124 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D77" t="e">
         <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="D78" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B79" s="2"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="4"/>
-      <c r="E79" t="s">
+      <c r="B80" s="2"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="4"/>
+      <c r="E80" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
-        <v>0</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="E80">
-        <f>POWER(2, 32+(1+3*32)*2)/EXP(2000*A80^2)</f>
-        <v>1.0783978666860256E+68</v>
-      </c>
-      <c r="F80" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="E81">
-        <f t="shared" ref="E81:E91" si="1">POWER(2, 32+(1+3*32)*2)/EXP(2000*A81^2)</f>
-        <v>2.2227436693499066E+59</v>
+        <f>POWER(2, 32+(1+3*32)*2)/EXP(2000*A81^2)</f>
+        <v>1.0783978666860256E+68</v>
       </c>
       <c r="F81" t="s">
-        <v>227</v>
+        <v>51</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="E82">
+        <f t="shared" ref="E82:E92" si="1">POWER(2, 32+(1+3*32)*2)/EXP(2000*A82^2)</f>
+        <v>2.2227436693499066E+59</v>
+      </c>
+      <c r="F82" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="E83">
         <f t="shared" si="1"/>
         <v>1.9463478863377805E+33</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F83" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>0.28199999999999997</v>
       </c>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1">
         <f t="shared" si="1"/>
         <v>9.101443183444155E-2</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+    <row r="85" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
         <v>0.3</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E85" s="2">
         <f t="shared" si="1"/>
         <v>7.2405620129442137E-11</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="E85">
-        <f t="shared" si="1"/>
-        <v>1.1443129452911475E-71</v>
-      </c>
-    </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="E86">
         <f t="shared" si="1"/>
+        <v>1.1443129452911475E-71</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="E87">
+        <f t="shared" si="1"/>
         <v>7.683127998071391E-150</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>0.6</v>
-      </c>
-      <c r="E87" t="e">
-        <f t="shared" si="1"/>
-        <v>#NUM!</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="E88" t="e">
         <f t="shared" si="1"/>
@@ -10325,7 +10942,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="E89" t="e">
         <f t="shared" si="1"/>
@@ -10334,7 +10951,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="E90" t="e">
         <f t="shared" si="1"/>
@@ -10343,9 +10960,18 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
+        <v>0.9</v>
+      </c>
+      <c r="E91" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
         <v>1</v>
       </c>
-      <c r="E91" t="e">
+      <c r="E92" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>

</xml_diff>

<commit_message>
Added confidence interval calculations for timing experiments
</commit_message>
<xml_diff>
--- a/hs/KP_Performance_Results.xlsx
+++ b/hs/KP_Performance_Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\MLCert\hs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF30570-F4FC-482C-B172-40B4FC7871CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EB8FBF-E64E-455F-B137-EDB3D5FF5B49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GenError" sheetId="1" r:id="rId1"/>
     <sheet name="GenErrorCalc" sheetId="2" r:id="rId2"/>
     <sheet name="Timing" sheetId="3" r:id="rId3"/>
+    <sheet name="TimingCalc" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="259">
   <si>
     <t>Data File Index</t>
   </si>
@@ -738,14 +739,87 @@
   </si>
   <si>
     <t>Synthetic Gen Err Run</t>
+  </si>
+  <si>
+    <t>KP_1</t>
+  </si>
+  <si>
+    <t>KP_2</t>
+  </si>
+  <si>
+    <t>KP_3</t>
+  </si>
+  <si>
+    <t>KP_4</t>
+  </si>
+  <si>
+    <t>KP_5</t>
+  </si>
+  <si>
+    <t>KP_Ave</t>
+  </si>
+  <si>
+    <t>KP_STD</t>
+  </si>
+  <si>
+    <t>KP_CI</t>
+  </si>
+  <si>
+    <t>KPB_1</t>
+  </si>
+  <si>
+    <t>KPB_2</t>
+  </si>
+  <si>
+    <t>KPB_3</t>
+  </si>
+  <si>
+    <t>KPB_4</t>
+  </si>
+  <si>
+    <t>KPB_5</t>
+  </si>
+  <si>
+    <t>KPB_Ave</t>
+  </si>
+  <si>
+    <t>KPB_STD</t>
+  </si>
+  <si>
+    <t>KPB_CI</t>
+  </si>
+  <si>
+    <t>KPD_1</t>
+  </si>
+  <si>
+    <t>KPD_2</t>
+  </si>
+  <si>
+    <t>KPD_3</t>
+  </si>
+  <si>
+    <t>KPD_4</t>
+  </si>
+  <si>
+    <t>KPD_5</t>
+  </si>
+  <si>
+    <t>KPD_Ave</t>
+  </si>
+  <si>
+    <t>KPD_STD</t>
+  </si>
+  <si>
+    <t>KPD_CI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -784,13 +858,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7908,8 +7983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9707,7 +9782,7 @@
         <v>27</v>
       </c>
       <c r="D85">
-        <f>_xlfn.CONFIDENCE.NORM(0.05,D82,20)</f>
+        <f>_xlfn.CONFIDENCE.NORM(0.05, D82,20)</f>
         <v>5.7948611332940842E-3</v>
       </c>
     </row>
@@ -10987,7 +11062,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11427,4 +11502,2489 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B9939-293C-4DC9-8D3A-5A6F24858279}">
+  <dimension ref="A1:AA25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="4" customWidth="1"/>
+    <col min="19" max="19" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>196.85</v>
+      </c>
+      <c r="C2">
+        <f>200.581</f>
+        <v>200.58099999999999</v>
+      </c>
+      <c r="D2">
+        <f>197.57</f>
+        <v>197.57</v>
+      </c>
+      <c r="E2">
+        <f>198.813</f>
+        <v>198.81299999999999</v>
+      </c>
+      <c r="F2">
+        <f>205.903</f>
+        <v>205.90299999999999</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(B2:F2)</f>
+        <v>199.9434</v>
+      </c>
+      <c r="H2">
+        <f>_xlfn.STDEV.S(B2:F2)</f>
+        <v>3.6195069139317853</v>
+      </c>
+      <c r="I2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, H2, 5)</f>
+        <v>3.1725793958339898</v>
+      </c>
+      <c r="K2">
+        <f>0.462</f>
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="L2">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M2">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N2">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="O2">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="P2">
+        <f>AVERAGE(K2:O2)</f>
+        <v>0.3498</v>
+      </c>
+      <c r="Q2">
+        <f>_xlfn.STDEV.S(K2:O2)</f>
+        <v>6.2731172474297242E-2</v>
+      </c>
+      <c r="R2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, Q2, 5)</f>
+        <v>5.4985286670518725E-2</v>
+      </c>
+      <c r="T2" s="6">
+        <f>0.409</f>
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="U2" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="V2" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W2" s="6">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X2" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Y2">
+        <f>AVERAGE(T2:X2)</f>
+        <v>0.29459999999999997</v>
+      </c>
+      <c r="Z2">
+        <f>_xlfn.STDEV.S(T2:X2)</f>
+        <v>6.3959362098132536E-2</v>
+      </c>
+      <c r="AA2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05,Z2,5)</f>
+        <v>5.6061822559912634E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>201.91200000000001</v>
+      </c>
+      <c r="C3">
+        <f>200.987</f>
+        <v>200.98699999999999</v>
+      </c>
+      <c r="D3">
+        <f>201.092</f>
+        <v>201.09200000000001</v>
+      </c>
+      <c r="E3">
+        <f>199.391</f>
+        <v>199.39099999999999</v>
+      </c>
+      <c r="F3">
+        <f>206.741</f>
+        <v>206.74100000000001</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G25" si="0">AVERAGE(B3:F3)</f>
+        <v>202.02459999999999</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H25" si="1">_xlfn.STDEV.S(B3:F3)</f>
+        <v>2.7901305166604735</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I25" si="2">_xlfn.CONFIDENCE.NORM(0.05, H3, 5)</f>
+        <v>2.4456122890034879</v>
+      </c>
+      <c r="K3">
+        <f>0.448</f>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="L3">
+        <f>0.317</f>
+        <v>0.317</v>
+      </c>
+      <c r="M3">
+        <f>0.319</f>
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="N3">
+        <f>0.316</f>
+        <v>0.316</v>
+      </c>
+      <c r="O3">
+        <f>0.318</f>
+        <v>0.318</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P25" si="3">AVERAGE(K3:O3)</f>
+        <v>0.34360000000000002</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q25" si="4">_xlfn.STDEV.S(K3:O3)</f>
+        <v>5.837208236820042E-2</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R25" si="5">_xlfn.CONFIDENCE.NORM(0.05, Q3, 5)</f>
+        <v>5.1164445936120496E-2</v>
+      </c>
+      <c r="T3" s="6">
+        <f>0.406</f>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="U3" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="V3" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="W3" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X3" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y25" si="6">AVERAGE(T3:X3)</f>
+        <v>0.29380000000000006</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z25" si="7">_xlfn.STDEV.S(T3:X3)</f>
+        <v>6.2735157607198E-2</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" ref="AA3:AA25" si="8">_xlfn.CONFIDENCE.NORM(0.05,Z3,5)</f>
+        <v>5.4988779729333435E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>202.428</v>
+      </c>
+      <c r="C4">
+        <f>200.622</f>
+        <v>200.62200000000001</v>
+      </c>
+      <c r="D4">
+        <f>200.622</f>
+        <v>200.62200000000001</v>
+      </c>
+      <c r="E4">
+        <f>199.999</f>
+        <v>199.999</v>
+      </c>
+      <c r="F4">
+        <f>207.716</f>
+        <v>207.71600000000001</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>202.2774</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>3.1730448783463503</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>2.7812453581316521</v>
+      </c>
+      <c r="K4">
+        <f>0.452</f>
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="L4">
+        <f>0.316</f>
+        <v>0.316</v>
+      </c>
+      <c r="M4">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N4">
+        <f>0.318</f>
+        <v>0.318</v>
+      </c>
+      <c r="O4">
+        <f>0.318</f>
+        <v>0.318</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>0.34500000000000003</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="4"/>
+        <v>5.9841457201508498E-2</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="5"/>
+        <v>5.2452386098070986E-2</v>
+      </c>
+      <c r="T4" s="6">
+        <f>0.406</f>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="U4" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="V4" s="6">
+        <f>0.263</f>
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="W4" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X4" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="6"/>
+        <v>0.29320000000000002</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="7"/>
+        <v>6.3076937148216189E-2</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" si="8"/>
+        <v>5.5288357200943793E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>199.584</v>
+      </c>
+      <c r="C5">
+        <f>199.628</f>
+        <v>199.62799999999999</v>
+      </c>
+      <c r="D5">
+        <f>199.387</f>
+        <v>199.387</v>
+      </c>
+      <c r="E5">
+        <f>199.64</f>
+        <v>199.64</v>
+      </c>
+      <c r="F5">
+        <f>206.264</f>
+        <v>206.26400000000001</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>200.9006</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>2.9999626331006262</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>2.6295348688001714</v>
+      </c>
+      <c r="K5">
+        <f>0.453</f>
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="L5">
+        <f>0.319</f>
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="M5">
+        <f>0.319</f>
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="N5">
+        <f>0.318</f>
+        <v>0.318</v>
+      </c>
+      <c r="O5">
+        <f>0.319</f>
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>0.34560000000000002</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="4"/>
+        <v>6.0039986675548315E-2</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="5"/>
+        <v>5.26264016570357E-2</v>
+      </c>
+      <c r="T5" s="6">
+        <f>0.405</f>
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="U5" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="V5" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W5" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="X5" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="6"/>
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="7"/>
+        <v>6.2076565626651925E-2</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="8"/>
+        <v>5.4411509013341824E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>202.048</v>
+      </c>
+      <c r="C6">
+        <f>199.581</f>
+        <v>199.58099999999999</v>
+      </c>
+      <c r="D6">
+        <f>198.762</f>
+        <v>198.762</v>
+      </c>
+      <c r="E6">
+        <f>202.233</f>
+        <v>202.233</v>
+      </c>
+      <c r="F6">
+        <f>207.436</f>
+        <v>207.43600000000001</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>202.012</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>3.3890328266335858</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>2.9705636632983032</v>
+      </c>
+      <c r="K6">
+        <f>0.456</f>
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="L6">
+        <f>0.318</f>
+        <v>0.318</v>
+      </c>
+      <c r="M6">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="N6">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="O6">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>0.34680000000000005</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="4"/>
+        <v>6.1050798520576176E-2</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="5"/>
+        <v>5.3512401023484424E-2</v>
+      </c>
+      <c r="T6" s="6">
+        <f>0.408</f>
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="U6" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="V6" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W6" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="X6" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="6"/>
+        <v>0.29459999999999997</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="7"/>
+        <v>6.3401892716227468E-2</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="8"/>
+        <v>5.5573188080991549E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>201.11799999999999</v>
+      </c>
+      <c r="C7">
+        <f>202.436</f>
+        <v>202.43600000000001</v>
+      </c>
+      <c r="D7">
+        <f>199.796</f>
+        <v>199.79599999999999</v>
+      </c>
+      <c r="E7">
+        <f>199.275</f>
+        <v>199.27500000000001</v>
+      </c>
+      <c r="F7">
+        <f>206.305</f>
+        <v>206.30500000000001</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>201.78599999999997</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>2.8087054847384798</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>2.4618936672143508</v>
+      </c>
+      <c r="K7">
+        <f>0.464</f>
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="L7">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M7">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N7">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="O7">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>0.35039999999999999</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="4"/>
+        <v>6.3508267178376432E-2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="5"/>
+        <v>5.5666427694806821E-2</v>
+      </c>
+      <c r="T7" s="6">
+        <f>0.41</f>
+        <v>0.41</v>
+      </c>
+      <c r="U7" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="V7" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="W7" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="X7" s="6">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="6"/>
+        <v>0.2944</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="7"/>
+        <v>6.4639771039198643E-2</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="8"/>
+        <v>5.6658216333566921E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>199.59100000000001</v>
+      </c>
+      <c r="C8">
+        <f>199.239</f>
+        <v>199.239</v>
+      </c>
+      <c r="D8">
+        <f>197.91</f>
+        <v>197.91</v>
+      </c>
+      <c r="E8">
+        <f>197.968</f>
+        <v>197.96799999999999</v>
+      </c>
+      <c r="F8">
+        <f>205.271</f>
+        <v>205.27099999999999</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>199.99579999999997</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>3.042485776466338</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>2.6668073624563875</v>
+      </c>
+      <c r="K8">
+        <f>0.454</f>
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="L8">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M8">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N8">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="O8">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>0.34839999999999999</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="4"/>
+        <v>5.9036429431326524E-2</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="5"/>
+        <v>5.1746761111716381E-2</v>
+      </c>
+      <c r="T8" s="6">
+        <f>0.404</f>
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="U8" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="V8" s="6">
+        <f>0.263</f>
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="W8" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="X8" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="6"/>
+        <v>0.29339999999999999</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="7"/>
+        <v>6.1853051662792126E-2</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="8"/>
+        <v>5.4215593985885088E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>200.32400000000001</v>
+      </c>
+      <c r="C9">
+        <f>199.908</f>
+        <v>199.90799999999999</v>
+      </c>
+      <c r="D9">
+        <f>198.839</f>
+        <v>198.839</v>
+      </c>
+      <c r="E9">
+        <f>200.583</f>
+        <v>200.583</v>
+      </c>
+      <c r="F9">
+        <f>207.621</f>
+        <v>207.62100000000001</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>201.45499999999998</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>3.5105471795718737</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>3.0770737326522908</v>
+      </c>
+      <c r="K9">
+        <f>0.466</f>
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="L9">
+        <f>0.325</f>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="M9">
+        <f>0.324</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="N9">
+        <f>0.326</f>
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="O9">
+        <f>0.325</f>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>0.35320000000000001</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="4"/>
+        <v>6.3061081500399491E-2</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="5"/>
+        <v>5.5274459368237015E-2</v>
+      </c>
+      <c r="T9" s="6">
+        <f>0.406</f>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="U9" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="V9" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="W9" s="6">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="X9" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="6"/>
+        <v>0.29500000000000004</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="7"/>
+        <v>6.2064482596731668E-2</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="8"/>
+        <v>5.4400917965258255E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>201.124</v>
+      </c>
+      <c r="C10">
+        <f>201.844</f>
+        <v>201.84399999999999</v>
+      </c>
+      <c r="D10">
+        <f>199.87</f>
+        <v>199.87</v>
+      </c>
+      <c r="E10">
+        <f>197.443</f>
+        <v>197.44300000000001</v>
+      </c>
+      <c r="F10">
+        <f>206.527</f>
+        <v>206.52699999999999</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>201.36160000000001</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3.3373199277264294</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>2.9252361417676225</v>
+      </c>
+      <c r="K10">
+        <f>0.46</f>
+        <v>0.46</v>
+      </c>
+      <c r="L10">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="M10">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N10">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="O10">
+        <f>0.319</f>
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>0.34820000000000001</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="4"/>
+        <v>6.2503599896325854E-2</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="5"/>
+        <v>5.4785814176309677E-2</v>
+      </c>
+      <c r="T10" s="6">
+        <f>0.407</f>
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="U10" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="V10" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="W10" s="6">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X10" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="6"/>
+        <v>0.29360000000000003</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="7"/>
+        <v>6.3405835693569848E-2</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="8"/>
+        <v>5.5576644189509125E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>202.56200000000001</v>
+      </c>
+      <c r="C11">
+        <f>200.011</f>
+        <v>200.011</v>
+      </c>
+      <c r="D11">
+        <f>200.402</f>
+        <v>200.40199999999999</v>
+      </c>
+      <c r="E11">
+        <f>201.503</f>
+        <v>201.50299999999999</v>
+      </c>
+      <c r="F11">
+        <f>208.253</f>
+        <v>208.25299999999999</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>202.54619999999994</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>3.3421892076900717</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>2.9295041754121329</v>
+      </c>
+      <c r="K11">
+        <f>0.459</f>
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="L11">
+        <f>0.324</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="M11">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N11">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="O11">
+        <f>0.324</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>0.35020000000000001</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="4"/>
+        <v>6.0833378995416437E-2</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="5"/>
+        <v>5.3321827908920448E-2</v>
+      </c>
+      <c r="T11" s="6">
+        <f>0.405</f>
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="U11" s="6">
+        <f>0.269</f>
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="V11" s="6">
+        <f>0.263</f>
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="W11" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X11" s="6">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="6"/>
+        <v>0.29380000000000006</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="7"/>
+        <v>6.2202893823358217E-2</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="8"/>
+        <v>5.4522238525265283E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>199.74600000000001</v>
+      </c>
+      <c r="C12">
+        <f>198.875</f>
+        <v>198.875</v>
+      </c>
+      <c r="D12">
+        <f>198.366</f>
+        <v>198.36600000000001</v>
+      </c>
+      <c r="E12">
+        <f>198.066</f>
+        <v>198.066</v>
+      </c>
+      <c r="F12">
+        <f>205.204</f>
+        <v>205.20400000000001</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>200.0514</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>2.9499516606208998</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>2.585699124145536</v>
+      </c>
+      <c r="K12">
+        <f>0.459</f>
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="L12">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="M12">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N12">
+        <f>0.324</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="O12">
+        <f>0.324</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>0.35020000000000001</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="4"/>
+        <v>6.0833378995416437E-2</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="5"/>
+        <v>5.3321827908920448E-2</v>
+      </c>
+      <c r="T12" s="6">
+        <f>0.405</f>
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="U12" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="V12" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W12" s="6">
+        <f>0.269</f>
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="X12" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="6"/>
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="7"/>
+        <v>6.1973381382654943E-2</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="8"/>
+        <v>5.4321065697646116E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>200.34299999999999</v>
+      </c>
+      <c r="C13">
+        <f>198.52</f>
+        <v>198.52</v>
+      </c>
+      <c r="D13">
+        <f>199.919</f>
+        <v>199.91900000000001</v>
+      </c>
+      <c r="E13">
+        <f>197.629</f>
+        <v>197.62899999999999</v>
+      </c>
+      <c r="F13">
+        <f>206.636</f>
+        <v>206.636</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>200.60939999999999</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>3.5396294015051897</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>3.1025649557068928</v>
+      </c>
+      <c r="K13">
+        <f>0.455</f>
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="L13">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="M13">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="N13">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="O13">
+        <f>0.324</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>0.34860000000000002</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="4"/>
+        <v>5.9492016271092775E-2</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="5"/>
+        <v>5.2146093245961547E-2</v>
+      </c>
+      <c r="T13" s="6">
+        <f>0.407</f>
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="U13" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="V13" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W13" s="6">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X13" s="6">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="6"/>
+        <v>0.29400000000000004</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="7"/>
+        <v>6.3174361888348088E-2</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="8"/>
+        <v>5.5373752181679219E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>200.13900000000001</v>
+      </c>
+      <c r="C14">
+        <f>201.385</f>
+        <v>201.38499999999999</v>
+      </c>
+      <c r="D14">
+        <f>197.294</f>
+        <v>197.29400000000001</v>
+      </c>
+      <c r="E14">
+        <f>197.214</f>
+        <v>197.214</v>
+      </c>
+      <c r="F14">
+        <f>206.362</f>
+        <v>206.36199999999999</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>200.47879999999998</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>3.7533509961100044</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>3.2898967507859833</v>
+      </c>
+      <c r="K14">
+        <f>0.458</f>
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="L14">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="M14">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="N14">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="O14">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="3"/>
+        <v>0.34920000000000001</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="4"/>
+        <v>6.0825159268184638E-2</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="5"/>
+        <v>5.3314623132724386E-2</v>
+      </c>
+      <c r="T14" s="6">
+        <f>0.41</f>
+        <v>0.41</v>
+      </c>
+      <c r="U14" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="V14" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="W14" s="6">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="X14" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="6"/>
+        <v>0.29480000000000001</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="7"/>
+        <v>6.4429806766744174E-2</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="8"/>
+        <v>5.6474177916044817E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>202.60400000000001</v>
+      </c>
+      <c r="C15">
+        <f>201.954</f>
+        <v>201.95400000000001</v>
+      </c>
+      <c r="D15">
+        <f>202.032</f>
+        <v>202.03200000000001</v>
+      </c>
+      <c r="E15">
+        <f>201.117</f>
+        <v>201.11699999999999</v>
+      </c>
+      <c r="F15">
+        <f>210.567</f>
+        <v>210.56700000000001</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>203.65479999999999</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>3.9002986680509499</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>3.4186996975274746</v>
+      </c>
+      <c r="K15">
+        <f>0.451</f>
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="L15">
+        <f>0.316</f>
+        <v>0.316</v>
+      </c>
+      <c r="M15">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N15">
+        <f>0.318</f>
+        <v>0.318</v>
+      </c>
+      <c r="O15">
+        <f>0.316</f>
+        <v>0.316</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>0.34440000000000004</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="4"/>
+        <v>5.9626336463009223E-2</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="5"/>
+        <v>5.2263827921830888E-2</v>
+      </c>
+      <c r="T15" s="6">
+        <f>0.402</f>
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="U15" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="V15" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W15" s="6">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="X15" s="6">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="6"/>
+        <v>0.29339999999999999</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="7"/>
+        <v>6.072314221118659E-2</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="8"/>
+        <v>5.3225202882742316E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>204.52600000000001</v>
+      </c>
+      <c r="C16">
+        <f>202.242</f>
+        <v>202.24199999999999</v>
+      </c>
+      <c r="D16">
+        <f>198.686</f>
+        <v>198.68600000000001</v>
+      </c>
+      <c r="E16">
+        <f>198.7</f>
+        <v>198.7</v>
+      </c>
+      <c r="F16">
+        <f>210.175</f>
+        <v>210.17500000000001</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>202.86579999999998</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>4.7800212551828745</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>4.1897963746029525</v>
+      </c>
+      <c r="K16">
+        <f>0.456</f>
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="L16">
+        <f>0.317</f>
+        <v>0.317</v>
+      </c>
+      <c r="M16">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N16">
+        <f>0.316</f>
+        <v>0.316</v>
+      </c>
+      <c r="O16">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="3"/>
+        <v>0.34620000000000001</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="4"/>
+        <v>6.1422308650847843E-2</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="5"/>
+        <v>5.3838038026720075E-2</v>
+      </c>
+      <c r="T16" s="6">
+        <f>0.406</f>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="U16" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="V16" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="W16" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X16" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="6"/>
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="7"/>
+        <v>6.262188115986303E-2</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="8"/>
+        <v>5.48894903699279E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>201.14</v>
+      </c>
+      <c r="C17">
+        <f>199.529</f>
+        <v>199.529</v>
+      </c>
+      <c r="D17">
+        <f>198.682</f>
+        <v>198.68199999999999</v>
+      </c>
+      <c r="E17">
+        <f>200.472</f>
+        <v>200.47200000000001</v>
+      </c>
+      <c r="F17">
+        <f>209.314</f>
+        <v>209.31399999999999</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>201.82739999999998</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>4.2876272925710319</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>3.7582019675298497</v>
+      </c>
+      <c r="K17">
+        <f>0.46</f>
+        <v>0.46</v>
+      </c>
+      <c r="L17">
+        <f>0.324</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="M17">
+        <f>0.363</f>
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="N17">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="O17">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="3"/>
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="4"/>
+        <v>5.9686681931566808E-2</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="5"/>
+        <v>5.2316722085243274E-2</v>
+      </c>
+      <c r="T17" s="6">
+        <f>0.409</f>
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="U17" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="V17" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W17" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="X17" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="6"/>
+        <v>0.29500000000000004</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="7"/>
+        <v>6.3737743919909898E-2</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="8"/>
+        <v>5.5867569231298972E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>200.815</v>
+      </c>
+      <c r="C18">
+        <f>196.99</f>
+        <v>196.99</v>
+      </c>
+      <c r="D18">
+        <f>200.107</f>
+        <v>200.107</v>
+      </c>
+      <c r="E18">
+        <f>197.42</f>
+        <v>197.42</v>
+      </c>
+      <c r="F18">
+        <f>207.804</f>
+        <v>207.804</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>200.62719999999999</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>4.3395763272467063</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>3.8037364673842728</v>
+      </c>
+      <c r="K18">
+        <f>0.458</f>
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="L18">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="M18">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N18">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="O18">
+        <f>0.324</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>0.34920000000000001</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="4"/>
+        <v>6.084159761216007E-2</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="5"/>
+        <v>5.332903171174861E-2</v>
+      </c>
+      <c r="T18" s="6">
+        <f>0.407</f>
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="U18" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="V18" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="W18" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="X18" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="6"/>
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="7"/>
+        <v>6.307297360993841E-2</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="8"/>
+        <v>5.5284883070302882E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>201.124</v>
+      </c>
+      <c r="C19">
+        <f>201.456</f>
+        <v>201.45599999999999</v>
+      </c>
+      <c r="D19">
+        <f>200.643</f>
+        <v>200.643</v>
+      </c>
+      <c r="E19">
+        <f>200.159</f>
+        <v>200.15899999999999</v>
+      </c>
+      <c r="F19">
+        <f>208.663</f>
+        <v>208.66300000000001</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>202.40899999999999</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>3.5303401394200038</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>3.0944227081039037</v>
+      </c>
+      <c r="K19">
+        <f>0.459</f>
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="L19">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="M19">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="N19">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="O19">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>0.34920000000000007</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="4"/>
+        <v>6.1389738556211382E-2</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="5"/>
+        <v>5.3809489604622507E-2</v>
+      </c>
+      <c r="T19" s="6">
+        <f>0.405</f>
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="U19" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="V19" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W19" s="6">
+        <f>0.267</f>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X19" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="6"/>
+        <v>0.29380000000000001</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="7"/>
+        <v>6.2182795048148283E-2</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="8"/>
+        <v>5.4504621495755794E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>200.642</v>
+      </c>
+      <c r="C20">
+        <f>199.833</f>
+        <v>199.833</v>
+      </c>
+      <c r="D20">
+        <f>199.627</f>
+        <v>199.62700000000001</v>
+      </c>
+      <c r="E20">
+        <f>199.624</f>
+        <v>199.624</v>
+      </c>
+      <c r="F20">
+        <f>206.29</f>
+        <v>206.29</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>201.20320000000001</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>2.8742915127036053</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>2.5193812990726689</v>
+      </c>
+      <c r="K20">
+        <f>0.458</f>
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="L20">
+        <f>0.319</f>
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="M20">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="N20">
+        <f>0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="O20">
+        <f>0.321</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>0.34760000000000002</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="4"/>
+        <v>6.1719526893844669E-2</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="5"/>
+        <v>5.4098556516177364E-2</v>
+      </c>
+      <c r="T20" s="6">
+        <f>0.409</f>
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="U20" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="V20" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="W20" s="6">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="X20" s="6">
+        <f>0.264</f>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="6"/>
+        <v>0.29380000000000001</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="7"/>
+        <v>6.4410402886490248E-2</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="8"/>
+        <v>5.6457169977627598E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>202.23599999999999</v>
+      </c>
+      <c r="C21">
+        <f>200.64</f>
+        <v>200.64</v>
+      </c>
+      <c r="D21">
+        <f>198.093</f>
+        <v>198.09299999999999</v>
+      </c>
+      <c r="E21">
+        <f>200.082</f>
+        <v>200.08199999999999</v>
+      </c>
+      <c r="F21">
+        <f>206.975</f>
+        <v>206.97499999999999</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>201.6052</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>3.347385502149403</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>2.9340588446332099</v>
+      </c>
+      <c r="K21">
+        <f>0.459</f>
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="L21">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M21">
+        <f>0.322</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="N21">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="O21">
+        <f>0.323</f>
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>0.3498</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="4"/>
+        <v>6.1046703432700009E-2</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="5"/>
+        <v>5.3508811586655318E-2</v>
+      </c>
+      <c r="T21" s="6">
+        <f>0.406</f>
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="U21" s="6">
+        <f>0.27</f>
+        <v>0.27</v>
+      </c>
+      <c r="V21" s="6">
+        <f>0.265</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="W21" s="6">
+        <f>0.268</f>
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="X21" s="6">
+        <f>0.266</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="6"/>
+        <v>0.29500000000000004</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="7"/>
+        <v>6.2080592780675105E-2</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="8"/>
+        <v>5.4415038904617512E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C22">
+        <f>0.085</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D22">
+        <f>0.085</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E22">
+        <f>0.085</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="F22">
+        <f>0.087</f>
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>8.7200000000000014E-2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>3.8987177379235832E-3</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>3.4173139766357609E-3</v>
+      </c>
+      <c r="K22">
+        <f>0.013</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="L22">
+        <f>0.003</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M22">
+        <f>0.003</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N22">
+        <f>0.003</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O22">
+        <f>0.003</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="3"/>
+        <v>4.9999999999999992E-3</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="4"/>
+        <v>4.4721359549995798E-3</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="5"/>
+        <v>3.9199279690801071E-3</v>
+      </c>
+      <c r="T22" s="6">
+        <f>0.013</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="U22" s="6">
+        <f>0.002</f>
+        <v>2E-3</v>
+      </c>
+      <c r="V22" s="6">
+        <f>0.002</f>
+        <v>2E-3</v>
+      </c>
+      <c r="W22" s="6">
+        <f>0.002</f>
+        <v>2E-3</v>
+      </c>
+      <c r="X22" s="6">
+        <f>0.002</f>
+        <v>2E-3</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="6"/>
+        <v>4.2000000000000006E-3</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="7"/>
+        <v>4.9193495504995348E-3</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="8"/>
+        <v>4.3119207659881153E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="C23">
+        <f>0.218</f>
+        <v>0.218</v>
+      </c>
+      <c r="D23">
+        <f>0.22</f>
+        <v>0.22</v>
+      </c>
+      <c r="E23">
+        <f>0.218</f>
+        <v>0.218</v>
+      </c>
+      <c r="F23">
+        <f>0.216</f>
+        <v>0.216</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0.22080000000000002</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>6.4187226143524916E-3</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>5.6261550531886018E-3</v>
+      </c>
+      <c r="K23">
+        <f>0.017</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="L23">
+        <f>0.006</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="M23">
+        <f>0.005</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N23">
+        <f>0.005</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O23">
+        <f>0.005</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="3"/>
+        <v>7.6E-3</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="4"/>
+        <v>5.2725705305856291E-3</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="5"/>
+        <v>4.6215269168381288E-3</v>
+      </c>
+      <c r="T23" s="6">
+        <f>0.017</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="U23" s="6">
+        <f>0.005</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="V23" s="6">
+        <f>0.004</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="W23" s="6">
+        <f>0.004</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="X23" s="6">
+        <f>0.004</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="6"/>
+        <v>6.8000000000000005E-3</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="7"/>
+        <v>5.7183913821983196E-3</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="8"/>
+        <v>5.0122989423357E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>1044.636</v>
+      </c>
+      <c r="C24">
+        <f>1046.609</f>
+        <v>1046.6089999999999</v>
+      </c>
+      <c r="D24">
+        <f>1047.802</f>
+        <v>1047.8019999999999</v>
+      </c>
+      <c r="E24">
+        <f>1046.586</f>
+        <v>1046.586</v>
+      </c>
+      <c r="F24">
+        <f>1043.563</f>
+        <v>1043.5630000000001</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>1045.8391999999999</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>1.7052611823412236</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>1.4946998638923541</v>
+      </c>
+      <c r="K24">
+        <f>83.226</f>
+        <v>83.225999999999999</v>
+      </c>
+      <c r="L24">
+        <f>78.271</f>
+        <v>78.271000000000001</v>
+      </c>
+      <c r="M24">
+        <f>78.045</f>
+        <v>78.045000000000002</v>
+      </c>
+      <c r="N24">
+        <f>77.998</f>
+        <v>77.998000000000005</v>
+      </c>
+      <c r="O24">
+        <f>77.599</f>
+        <v>77.599000000000004</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="3"/>
+        <v>79.027799999999999</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="4"/>
+        <v>2.3593157270700313</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="5"/>
+        <v>2.0679934151137078</v>
+      </c>
+      <c r="T24" s="6">
+        <f>68.773</f>
+        <v>68.772999999999996</v>
+      </c>
+      <c r="U24" s="6">
+        <f>65.812</f>
+        <v>65.811999999999998</v>
+      </c>
+      <c r="V24" s="6">
+        <f>65.477</f>
+        <v>65.477000000000004</v>
+      </c>
+      <c r="W24" s="6">
+        <f>65.397</f>
+        <v>65.397000000000006</v>
+      </c>
+      <c r="X24" s="6">
+        <f>65.385</f>
+        <v>65.385000000000005</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="6"/>
+        <v>66.168800000000005</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="7"/>
+        <v>1.466097609301642</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="8"/>
+        <v>1.2850676012383273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>2120.556</v>
+      </c>
+      <c r="C25">
+        <f>2123.456</f>
+        <v>2123.4560000000001</v>
+      </c>
+      <c r="D25">
+        <f>2126.547</f>
+        <v>2126.547</v>
+      </c>
+      <c r="E25">
+        <f>2127.52</f>
+        <v>2127.52</v>
+      </c>
+      <c r="F25">
+        <f>2109.276</f>
+        <v>2109.2759999999998</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>2121.4710000000005</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>7.3459453442018674</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>6.43888667603653</v>
+      </c>
+      <c r="K25">
+        <f>146.986</f>
+        <v>146.98599999999999</v>
+      </c>
+      <c r="L25">
+        <f>136.707</f>
+        <v>136.70699999999999</v>
+      </c>
+      <c r="M25">
+        <f>136.165</f>
+        <v>136.16499999999999</v>
+      </c>
+      <c r="N25">
+        <f>136.848</f>
+        <v>136.84800000000001</v>
+      </c>
+      <c r="O25">
+        <f>136.622</f>
+        <v>136.62200000000001</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="3"/>
+        <v>138.66559999999998</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="4"/>
+        <v>4.6582760008397903</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="5"/>
+        <v>4.0830839149630096</v>
+      </c>
+      <c r="T25" s="6">
+        <f>127.937</f>
+        <v>127.937</v>
+      </c>
+      <c r="U25" s="6">
+        <f>120.138</f>
+        <v>120.13800000000001</v>
+      </c>
+      <c r="V25" s="6">
+        <f>120.142</f>
+        <v>120.142</v>
+      </c>
+      <c r="W25" s="6">
+        <f>120.378</f>
+        <v>120.378</v>
+      </c>
+      <c r="X25" s="6">
+        <v>119.71299999999999</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="6"/>
+        <v>121.66159999999999</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="7"/>
+        <v>3.5162429239175155</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="8"/>
+        <v>3.0820661809566072</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D23 K19:K20 L11 M4 M9 M13 N18 N5 N16 O15 M2 U5:V5 U13 U16:U17 V8 V14 V16:W16 V18:V19 V20 W12 V2:V3" formula="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>